<commit_message>
week 1 of second course
</commit_message>
<xml_diff>
--- a/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/W1-V3 Linking Workbooks/W1_ExpensesQ1.xlsx
+++ b/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/W1-V3 Linking Workbooks/W1_ExpensesQ1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nic\Documents\Freelance Training\Maquarie Uni\MOOCS\Course2\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\Excel Skills for Business Intermediate I\Week 1\W1-V3 Linking Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627EDBBE-FADD-420F-B5BF-9354DB27ED59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="43" windowWidth="37397" windowHeight="15994" activeTab="2"/>
+    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="12384" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uma" sheetId="5" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="WeekEnding" localSheetId="0">Uma!$C$3</definedName>
     <definedName name="WeekEnding">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -132,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -503,15 +504,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Do Not Type" xfId="4"/>
+    <cellStyle name="Do Not Type" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="9" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input Custom" xfId="2"/>
-    <cellStyle name="Instructions" xfId="5"/>
+    <cellStyle name="Input Custom" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Instructions" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Table Totals" xfId="3"/>
+    <cellStyle name="Table Totals" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="3">
@@ -562,7 +563,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Expense Report" defaultPivotStyle="PivotStyleLight15">
-    <tableStyle name="Expense Report" pivot="0" count="3">
+    <tableStyle name="Expense Report" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
       <tableStyleElement type="lastColumn" dxfId="0"/>
@@ -888,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -899,16 +900,16 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
@@ -920,8 +921,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -929,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -937,7 +938,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -954,7 +955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -966,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -978,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -990,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1065,14 +1066,14 @@
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1081,7 +1082,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>127.34</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1152,14 +1153,14 @@
         <v>127.34</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1168,7 +1169,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>213.38</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>957.44</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>227.70000000000002</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -1251,14 +1252,14 @@
         <v>1398.5200000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -1279,14 +1280,14 @@
         <v>1900.8600000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -1301,7 +1302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="6"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1312,16 +1313,16 @@
       <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
@@ -1333,8 +1334,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>568.16000000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>63.320000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1499,14 +1500,14 @@
         <v>776.48000000000013</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +1516,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>65.760000000000005</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>435.31999999999994</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1590,14 +1591,14 @@
         <v>501.07999999999993</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1606,7 +1607,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1632,7 +1633,7 @@
         <v>77.650000000000006</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>268.79999999999995</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -1683,14 +1684,14 @@
         <v>346.44999999999993</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -1711,14 +1712,14 @@
         <v>1624.0099999999998</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -1733,7 +1734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1744,16 +1745,16 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>27</v>
       </c>
@@ -1765,8 +1766,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1841,7 +1842,7 @@
         <v>568.16000000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>63.320000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1967,14 +1968,14 @@
         <v>1151.48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1983,7 +1984,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>193.10000000000002</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>435.31999999999994</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -2088,14 +2089,14 @@
         <v>628.41999999999996</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -2104,7 +2105,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>213.38</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>1035.0900000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>496.5</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -2209,14 +2210,14 @@
         <v>1744.9700000000003</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -2237,14 +2238,14 @@
         <v>3524.8700000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>

</xml_diff>